<commit_message>
ajouter tâches dans outils de planif
</commit_message>
<xml_diff>
--- a/doc/B65_-_Hiver_2019_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/doc/B65_-_Hiver_2019_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecole\synthese\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecole\synthese\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7554DCE-A130-4617-B874-B6B66D2DE0F4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B567E58E-80F3-4CB6-890E-C401E05EDDB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,6 +50,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>jcdemers</author>
+    <author>Zenon Roy</author>
   </authors>
   <commentList>
     <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
@@ -106,12 +107,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C15" authorId="1" shapeId="0" xr:uid="{48520787-5FFC-4AA7-8D6E-0C18D2C3ADC5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Zenon Roy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+données bidons mais assez pour faire mettre en place le système</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="97">
   <si>
     <t>No</t>
   </si>
@@ -135,9 +160,6 @@
   </si>
   <si>
     <t>Rédaction du document de planification</t>
-  </si>
-  <si>
-    <t>Nom du projet super cool que vous faites!</t>
   </si>
   <si>
     <t>Prédéces.</t>
@@ -391,6 +413,72 @@
   <si>
     <t>Zénon Roy</t>
   </si>
+  <si>
+    <t>Configurer le serveur</t>
+  </si>
+  <si>
+    <t>Configurer Nuxt</t>
+  </si>
+  <si>
+    <t>Écrire un script pour populer la base de données</t>
+  </si>
+  <si>
+    <t>Mettre en place l'API</t>
+  </si>
+  <si>
+    <t>Calculatrice de statistiques d'items pour le jeu Borderlands 2</t>
+  </si>
+  <si>
+    <t>Calcul des statistiques</t>
+  </si>
+  <si>
+    <t>Faire la page sélection des pièces</t>
+  </si>
+  <si>
+    <t>Faire la page détails d'une pièce</t>
+  </si>
+  <si>
+    <t>Faire la page pour les stats de base d'un item</t>
+  </si>
+  <si>
+    <t>Faire le layout par défaut pour Nuxt</t>
+  </si>
+  <si>
+    <t>Faire la page liste des pièces/items</t>
+  </si>
+  <si>
+    <t>Exporter les vraies données du jeu et importer dans bd</t>
+  </si>
+  <si>
+    <t>Rédiger le rapport de projet</t>
+  </si>
+  <si>
+    <t>Rédiger le fichier Lisez_moi.txt</t>
+  </si>
+  <si>
+    <t>Réaliser le site web de présentation</t>
+  </si>
+  <si>
+    <t>Réaliser la vidéo de présentation</t>
+  </si>
+  <si>
+    <t>Faire une page détails fabriquant</t>
+  </si>
+  <si>
+    <t>Ajouter les boucliers comme type d'item</t>
+  </si>
+  <si>
+    <t>ajouter les grenades comme type d'item</t>
+  </si>
+  <si>
+    <t>Ajouter les reliques comme type d'item</t>
+  </si>
+  <si>
+    <t>Ajouter les class mods comme type d'item</t>
+  </si>
+  <si>
+    <t>Ajouter les items uniques</t>
+  </si>
 </sst>
 </file>
 
@@ -399,7 +487,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -603,6 +691,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -2654,10 +2755,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2731,10 +2832,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3077,10 +3178,10 @@
                   <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>29.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3576,10 +3677,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3693,10 +3794,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4032,13 +4133,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4155,10 +4256,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6676,6 +6777,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Zenon Roy" id="{EB64C2B9-0E44-451B-B8BD-E1ED3D375A77}" userId="ee13738c5b9085ac" providerId="Windows Live"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
@@ -6942,7 +7049,7 @@
   <dimension ref="B1:AJ90"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6963,7 +7070,7 @@
     <row r="1" spans="2:31" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:31" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="120" t="s">
-        <v>8</v>
+        <v>79</v>
       </c>
       <c r="C2" s="120"/>
       <c r="D2" s="120"/>
@@ -6974,14 +7081,14 @@
     </row>
     <row r="3" spans="2:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E3" s="121" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F3" s="121"/>
       <c r="G3" s="121"/>
@@ -6998,7 +7105,7 @@
     </row>
     <row r="5" spans="2:31" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="28"/>
@@ -7007,7 +7114,7 @@
       <c r="G5" s="28"/>
       <c r="H5" s="59" t="str">
         <f>IF(L44=0,CONCATENATE(AE12, " totalisant ", AE15, " de travail estimé."),CONCATENATE("Attention, il reste " &amp; L45 &amp; " à remplir."))</f>
-        <v>4 tâches ont été définies totalisant 12 heures et 30 minutes de travail estimé.</v>
+        <v>25 tâches ont été définies totalisant 69 heures et 45 minutes de travail estimé.</v>
       </c>
     </row>
     <row r="6" spans="2:31" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -7016,25 +7123,25 @@
         <v>0</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="65" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="65" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="65" t="s">
+      <c r="H7" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="68" t="s">
+      <c r="T7" s="7" t="s">
         <v>11</v>
-      </c>
-      <c r="T7" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
@@ -7045,10 +7152,10 @@
         <v>4</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F8" s="14">
         <v>1</v>
@@ -7080,7 +7187,7 @@
         <v>0</v>
       </c>
       <c r="R8" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S8" s="22">
         <v>233</v>
@@ -7090,10 +7197,10 @@
       </c>
       <c r="U8" s="3">
         <f>MAX(B8:B42)</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="W8" s="3">
         <v>1</v>
@@ -7103,7 +7210,7 @@
       </c>
       <c r="Y8" s="8">
         <f>MAX(G8:G42)</f>
-        <v>0.25</v>
+        <v>0.29166666666666702</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>1</v>
@@ -7116,11 +7223,11 @@
       </c>
       <c r="AC8" s="4">
         <f>COUNTA(C8:C43)</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="AD8" s="9">
         <f>SUM(G8:G43)</f>
-        <v>0.5208333333333337</v>
+        <v>2.9062500000000009</v>
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
@@ -7135,7 +7242,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="16">
         <v>1</v>
@@ -7167,7 +7274,7 @@
         <v>0</v>
       </c>
       <c r="R9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S9" s="22">
         <v>238</v>
@@ -7176,7 +7283,7 @@
         <v>2</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W9" s="3">
         <v>2</v>
@@ -7195,7 +7302,7 @@
       </c>
       <c r="AD9" s="10">
         <f>AD8</f>
-        <v>0.5208333333333337</v>
+        <v>2.9062500000000009</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
@@ -7210,7 +7317,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10" s="18">
         <v>2</v>
@@ -7242,7 +7349,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S10" s="22">
         <v>243</v>
@@ -7267,7 +7374,7 @@
       </c>
       <c r="AD10" s="62">
         <f>DAY(AD8)*24+HOUR(AD8)</f>
-        <v>12</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="2:31" x14ac:dyDescent="0.25">
@@ -7282,7 +7389,7 @@
         <v>3</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F11" s="16">
         <v>2</v>
@@ -7326,20 +7433,32 @@
       </c>
       <c r="AD11" s="4">
         <f>MINUTE(AD8)</f>
-        <v>30</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="43" t="str">
+      <c r="B12" s="43">
         <f t="shared" ref="B12:B42" si="5">IF(LEN(C12)&lt;&gt;0,IF(OR(LEN(B11)=0,B11="^"),"^",B11+1),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="41"/>
+        <v>5</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="19">
+        <v>4</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="18">
+        <v>1</v>
+      </c>
+      <c r="G12" s="31">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="L12" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7361,7 +7480,7 @@
         <v>0</v>
       </c>
       <c r="R12" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S12" s="22">
         <v>212</v>
@@ -7376,50 +7495,62 @@
         <v>0.2</v>
       </c>
       <c r="AC12" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AD12" s="4">
         <f>AC8</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="AE12" s="4" t="str">
         <f>AD12 &amp; " " &amp; AC12 &amp; IF(AD12 &gt; 1, "s ont été définies", " a été définie")</f>
-        <v>4 tâches ont été définies</v>
+        <v>25 tâches ont été définies</v>
       </c>
     </row>
     <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="44" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="30"/>
-      <c r="H13" s="40"/>
+      <c r="B13" s="44">
+        <f>IF(LEN(C13)&lt;&gt;0,IF(OR(LEN(B12)=0,B12="^"),"^",B12+1),"")</f>
+        <v>6</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="16">
+        <v>5</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+      <c r="G13" s="30">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="L13" s="3" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(NOT(ISBLANK($C13)),LEN(D13)=0)</f>
         <v>0</v>
       </c>
       <c r="M13" s="3" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(ISBLANK($C13)),LEN(E13)=0)</f>
         <v>0</v>
       </c>
       <c r="N13" s="3" t="b">
-        <f t="shared" si="2"/>
+        <f>AND(NOT(ISBLANK($C13)),LEN(F13)=0)</f>
         <v>0</v>
       </c>
       <c r="O13" s="3" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(ISBLANK($C13)),LEN(G13)=0)</f>
         <v>0</v>
       </c>
       <c r="P13" s="3" t="b">
-        <f t="shared" si="4"/>
+        <f>AND(NOT(ISBLANK($C13)),LEN(H13)=0)</f>
         <v>0</v>
       </c>
       <c r="R13" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S13" s="22">
         <v>222</v>
@@ -7434,28 +7565,40 @@
         <v>0.25</v>
       </c>
       <c r="AC13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AD13" s="4">
         <f>AD10</f>
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="AE13" s="4" t="str">
         <f>AD13 &amp; " " &amp; AC13 &amp; IF(AD13 &gt; 1, "s", "")</f>
-        <v>12 heures</v>
+        <v>69 heures</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="str">
+      <c r="B14" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="41"/>
+        <v>7</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="19">
+        <v>5</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="18">
+        <v>1</v>
+      </c>
+      <c r="G14" s="31">
+        <v>6.25E-2</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="L14" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7477,7 +7620,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S14" s="22">
         <v>232</v>
@@ -7492,28 +7635,40 @@
         <v>0.3</v>
       </c>
       <c r="AC14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="AD14" s="4">
         <f>AD11</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AE14" s="4" t="str">
         <f>AD14 &amp; " " &amp; AC14 &amp; IF(AD14 &gt; 1, "s", "")</f>
-        <v>30 minutes</v>
+        <v>45 minutes</v>
       </c>
     </row>
     <row r="15" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B15" s="44" t="str">
+      <c r="B15" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="40"/>
+        <v>8</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="16">
+        <v>6</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="16">
+        <v>3</v>
+      </c>
+      <c r="G15" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="L15" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7545,42 +7700,54 @@
       </c>
       <c r="AE15" s="4" t="str">
         <f>IF(AD13&gt;0,IF(AD14&gt;0,AE13&amp;" et "&amp;AE14,AE13),AE14)</f>
-        <v>12 heures et 30 minutes</v>
+        <v>69 heures et 45 minutes</v>
       </c>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="41"/>
+      <c r="B16" s="43">
+        <f>IF(LEN(C16)&lt;&gt;0,IF(OR(LEN(B15)=0,B15="^"),"^",B15+1),"")</f>
+        <v>9</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="18">
+        <v>8</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="18">
+        <v>3</v>
+      </c>
+      <c r="G16" s="31">
+        <v>0.29166666666666702</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="L16" s="3" t="b">
-        <f t="shared" si="0"/>
+        <f>AND(NOT(ISBLANK($C16)),LEN(D16)=0)</f>
         <v>0</v>
       </c>
       <c r="M16" s="3" t="b">
-        <f t="shared" si="1"/>
+        <f>AND(NOT(ISBLANK($C16)),LEN(E16)=0)</f>
         <v>0</v>
       </c>
       <c r="N16" s="3" t="b">
-        <f t="shared" si="2"/>
+        <f>AND(NOT(ISBLANK($C16)),LEN(F16)=0)</f>
         <v>0</v>
       </c>
       <c r="O16" s="3" t="b">
-        <f t="shared" si="3"/>
+        <f>AND(NOT(ISBLANK($C16)),LEN(G16)=0)</f>
         <v>0</v>
       </c>
       <c r="P16" s="3" t="b">
-        <f t="shared" si="4"/>
+        <f>AND(NOT(ISBLANK($C16)),LEN(H16)=0)</f>
         <v>0</v>
       </c>
       <c r="R16" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S16" s="22">
         <v>58</v>
@@ -7596,16 +7763,28 @@
       </c>
     </row>
     <row r="17" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B17" s="44" t="str">
+      <c r="B17" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="40"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="16">
+        <v>14</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="16">
+        <v>3</v>
+      </c>
+      <c r="G17" s="30">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="L17" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7627,7 +7806,7 @@
         <v>0</v>
       </c>
       <c r="R17" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S17" s="22">
         <v>82</v>
@@ -7670,16 +7849,28 @@
       </c>
     </row>
     <row r="18" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="str">
+      <c r="B18" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="41"/>
+        <v>11</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D18" s="18">
+        <v>14</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="18">
+        <v>3</v>
+      </c>
+      <c r="G18" s="31">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="L18" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7701,7 +7892,7 @@
         <v>0</v>
       </c>
       <c r="R18" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="S18" s="22">
         <v>106</v>
@@ -7720,40 +7911,52 @@
       </c>
       <c r="AD18" s="4">
         <f t="array" ref="AD18">SUM(($H$8:$H$42=$AC18)*$G$8:$G$42)</f>
-        <v>0</v>
+        <v>1.2291666666666663</v>
       </c>
       <c r="AE18" s="4">
         <f>AD18 * 24*60</f>
-        <v>0</v>
+        <v>1769.9999999999995</v>
       </c>
       <c r="AF18" s="4">
         <f t="shared" ref="AF18:AF19" si="6">DAY(AD18)*24+HOUR(AD18)</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="AG18" s="4">
         <f t="shared" ref="AG18:AG19" si="7">MINUTE(AD18)</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AH18" s="4" t="str">
         <f t="shared" ref="AH18:AH19" si="8">AF18&amp;"h"&amp;TEXT(AG18,"00")</f>
-        <v>0h00</v>
+        <v>29h30</v>
       </c>
       <c r="AJ18" s="4">
         <f>COUNTIF($H$8:$H$42,AC18)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B19" s="44" t="str">
+      <c r="B19" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C19" s="15"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="40"/>
+        <v>12</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="16">
+        <v>14</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="16">
+        <v>2</v>
+      </c>
+      <c r="G19" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="H19" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="L19" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7788,40 +7991,52 @@
       </c>
       <c r="AD19" s="4">
         <f t="array" ref="AD19">SUM(($H$8:$H$42=$AC19)*$G$8:$G$42)</f>
-        <v>0</v>
+        <v>1.1562500000000004</v>
       </c>
       <c r="AE19" s="4">
         <f>AD19 * 24*60</f>
-        <v>0</v>
+        <v>1665.0000000000007</v>
       </c>
       <c r="AF19" s="4">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="AG19" s="4">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="AH19" s="4" t="str">
         <f t="shared" si="8"/>
-        <v>0h00</v>
+        <v>27h45</v>
       </c>
       <c r="AJ19" s="4">
         <f>COUNTIF($H$8:$H$42,AC19)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="str">
+      <c r="B20" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="41"/>
+        <v>13</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D20" s="19">
+        <v>14</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="18">
+        <v>2</v>
+      </c>
+      <c r="G20" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>2</v>
+      </c>
       <c r="L20" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7854,16 +8069,28 @@
       </c>
     </row>
     <row r="21" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B21" s="44" t="str">
+      <c r="B21" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="30"/>
-      <c r="H21" s="40"/>
+        <v>14</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="16">
+        <v>5</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+      <c r="G21" s="30">
+        <v>4.1666666666666699E-2</v>
+      </c>
+      <c r="H21" s="40" t="s">
+        <v>2</v>
+      </c>
       <c r="L21" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7895,36 +8122,48 @@
       </c>
       <c r="AD21" s="4">
         <f>SUM(AD17:AD19)</f>
-        <v>0.5208333333333337</v>
+        <v>2.9062500000000004</v>
       </c>
       <c r="AE21" s="4">
         <f t="shared" ref="AE21" si="9">AD21 * 24*60</f>
-        <v>750.00000000000057</v>
+        <v>4185.0000000000009</v>
       </c>
       <c r="AF21" s="4">
         <f t="shared" ref="AF21" si="10">DAY(AD21)*24+HOUR(AD21)</f>
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="AG21" s="4">
         <f t="shared" ref="AG21" si="11">MINUTE(AD21)</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="AH21" s="4" t="str">
         <f t="shared" ref="AH21" si="12">AF21&amp;"h"&amp;TEXT(AG21,"00")</f>
-        <v>12h30</v>
+        <v>69h45</v>
       </c>
     </row>
     <row r="22" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="str">
+      <c r="B22" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C22" s="17"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="41"/>
+        <v>15</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="18">
+        <v>8</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="18">
+        <v>3</v>
+      </c>
+      <c r="G22" s="31">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>3</v>
+      </c>
       <c r="L22" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7956,16 +8195,28 @@
       </c>
     </row>
     <row r="23" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="str">
+      <c r="B23" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="30"/>
-      <c r="H23" s="40"/>
+        <v>16</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="16">
+        <v>13</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="16">
+        <v>1</v>
+      </c>
+      <c r="G23" s="30">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H23" s="40" t="s">
+        <v>3</v>
+      </c>
       <c r="L23" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -7997,16 +8248,28 @@
       </c>
     </row>
     <row r="24" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="str">
+      <c r="B24" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="41"/>
+        <v>17</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="19">
+        <v>13</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="18">
+        <v>1</v>
+      </c>
+      <c r="G24" s="31">
+        <v>2.0833333333333301E-2</v>
+      </c>
+      <c r="H24" s="41" t="s">
+        <v>3</v>
+      </c>
       <c r="L24" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8038,16 +8301,28 @@
       </c>
     </row>
     <row r="25" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B25" s="44" t="str">
+      <c r="B25" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="30"/>
-      <c r="H25" s="40"/>
+        <v>18</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="16">
+        <v>13</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+      <c r="G25" s="30">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H25" s="40" t="s">
+        <v>3</v>
+      </c>
       <c r="L25" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8079,16 +8354,28 @@
       </c>
     </row>
     <row r="26" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B26" s="43" t="str">
+      <c r="B26" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C26" s="17"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="41"/>
+        <v>19</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="D26" s="19">
+        <v>13</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="18">
+        <v>2</v>
+      </c>
+      <c r="G26" s="31">
+        <v>8.3333333333333301E-2</v>
+      </c>
+      <c r="H26" s="41" t="s">
+        <v>3</v>
+      </c>
       <c r="L26" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8120,16 +8407,28 @@
       </c>
     </row>
     <row r="27" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B27" s="44" t="str">
+      <c r="B27" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="30"/>
-      <c r="H27" s="40"/>
+        <v>20</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="16">
+        <v>13</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2</v>
+      </c>
+      <c r="G27" s="30">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="H27" s="40" t="s">
+        <v>3</v>
+      </c>
       <c r="L27" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8161,16 +8460,28 @@
       </c>
     </row>
     <row r="28" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B28" s="43" t="str">
+      <c r="B28" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C28" s="17"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="41"/>
+        <v>21</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D28" s="18">
+        <v>13</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="18">
+        <v>2</v>
+      </c>
+      <c r="G28" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="H28" s="41" t="s">
+        <v>3</v>
+      </c>
       <c r="L28" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8202,16 +8513,28 @@
       </c>
     </row>
     <row r="29" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B29" s="44" t="str">
+      <c r="B29" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="40"/>
+        <v>22</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="16">
+        <v>13</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="16">
+        <v>2</v>
+      </c>
+      <c r="G29" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="H29" s="40" t="s">
+        <v>3</v>
+      </c>
       <c r="L29" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8240,16 +8563,28 @@
       </c>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B30" s="43" t="str">
+      <c r="B30" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C30" s="17"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="41"/>
+        <v>23</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="19">
+        <v>13</v>
+      </c>
+      <c r="E30" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="18">
+        <v>2</v>
+      </c>
+      <c r="G30" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="H30" s="41" t="s">
+        <v>3</v>
+      </c>
       <c r="L30" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8278,16 +8613,28 @@
       </c>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B31" s="44" t="str">
+      <c r="B31" s="44">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="30"/>
-      <c r="H31" s="40"/>
+        <v>24</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="16">
+        <v>13</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="16">
+        <v>2</v>
+      </c>
+      <c r="G31" s="30">
+        <v>0.125</v>
+      </c>
+      <c r="H31" s="40" t="s">
+        <v>3</v>
+      </c>
       <c r="L31" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -8316,16 +8663,28 @@
       </c>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B32" s="43" t="str">
+      <c r="B32" s="43">
         <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="C32" s="17"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="41"/>
+        <v>25</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="19">
+        <v>13</v>
+      </c>
+      <c r="E32" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="18">
+        <v>2</v>
+      </c>
+      <c r="G32" s="31">
+        <v>0.125</v>
+      </c>
+      <c r="H32" s="41" t="s">
+        <v>3</v>
+      </c>
       <c r="L32" s="3" t="b">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -9169,7 +9528,7 @@
       <formula>LEN($B12)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="7">
+  <dataValidations xWindow="1071" yWindow="645" count="7">
     <dataValidation type="textLength" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Nom de tâche trop long" error="Le nom de votre tâche doit être court. _x000a_Un maximum de 72 caractères est mis à votre disposition._x000a_Pour plus de détail, veuillez faire l'ajout de commentaires." promptTitle="Nom de la tâche" prompt="_x000a_Veuillez saisir le nom de la tâche._x000a__x000a_Lorsque pertinent, n'oubliez pas d'ajouter une description de votre tâche sous forme de commentaire." sqref="C8:C42" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>0</formula1>
       <formula2>72</formula2>
@@ -9290,7 +9649,7 @@
     <row r="2" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="122" t="str">
         <f>'Sprint 1 - Planification'!B2:H2</f>
-        <v>Nom du projet super cool que vous faites!</v>
+        <v>Calculatrice de statistiques d'items pour le jeu Borderlands 2</v>
       </c>
       <c r="C2" s="122"/>
       <c r="D2" s="122"/>
@@ -9300,7 +9659,7 @@
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="32"/>
@@ -9318,7 +9677,7 @@
     </row>
     <row r="5" spans="2:23" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -9335,19 +9694,19 @@
         <v>0</v>
       </c>
       <c r="C7" s="66" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="67" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="68" t="s">
         <v>23</v>
-      </c>
-      <c r="G7" s="68" t="s">
-        <v>24</v>
       </c>
       <c r="K7" s="7"/>
     </row>
@@ -9520,17 +9879,17 @@
       </c>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="52" t="str">
+      <c r="B12" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B12)&lt;&gt;0,'Sprint 1 - Planification'!B12,"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="C12" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C12)&lt;&gt;0,'Sprint 1 - Planification'!C12,"")</f>
-        <v/>
+        <v>Configurer le serveur</v>
       </c>
       <c r="D12" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H12)&lt;&gt;0,'Sprint 1 - Planification'!H12,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E12" s="116"/>
       <c r="F12" s="114"/>
@@ -9549,7 +9908,7 @@
       </c>
       <c r="P12" s="8"/>
       <c r="S12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T12" s="62">
         <f>T10</f>
@@ -9561,17 +9920,17 @@
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="49" t="str">
+      <c r="B13" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B13)&lt;&gt;0,'Sprint 1 - Planification'!B13,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="C13" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C13)&lt;&gt;0,'Sprint 1 - Planification'!C13,"")</f>
-        <v/>
+        <v>Mettre en place l'API</v>
       </c>
       <c r="D13" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E13" s="110"/>
       <c r="F13" s="111"/>
@@ -9590,7 +9949,7 @@
       </c>
       <c r="P13" s="8"/>
       <c r="S13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="T13" s="4">
         <f>T11</f>
@@ -9602,17 +9961,17 @@
       </c>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B14" s="52" t="str">
+      <c r="B14" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B14)&lt;&gt;0,'Sprint 1 - Planification'!B14,"")</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="C14" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C14)&lt;&gt;0,'Sprint 1 - Planification'!C14,"")</f>
-        <v/>
+        <v>Configurer Nuxt</v>
       </c>
       <c r="D14" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E14" s="116"/>
       <c r="F14" s="114"/>
@@ -9640,17 +9999,17 @@
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="str">
+      <c r="B15" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B15)&lt;&gt;0,'Sprint 1 - Planification'!B15,"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="C15" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C15)&lt;&gt;0,'Sprint 1 - Planification'!C15,"")</f>
-        <v/>
+        <v>Écrire un script pour populer la base de données</v>
       </c>
       <c r="D15" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E15" s="110"/>
       <c r="F15" s="111"/>
@@ -9678,17 +10037,17 @@
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B16" s="52" t="str">
+      <c r="B16" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B16)&lt;&gt;0,'Sprint 1 - Planification'!B16,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="C16" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C16)&lt;&gt;0,'Sprint 1 - Planification'!C16,"")</f>
-        <v/>
+        <v>Calcul des statistiques</v>
       </c>
       <c r="D16" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E16" s="113"/>
       <c r="F16" s="114"/>
@@ -9708,17 +10067,17 @@
       <c r="P16" s="8"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17" s="49" t="str">
+      <c r="B17" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B17)&lt;&gt;0,'Sprint 1 - Planification'!B17,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="C17" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C17)&lt;&gt;0,'Sprint 1 - Planification'!C17,"")</f>
-        <v/>
+        <v>Faire la page sélection des pièces</v>
       </c>
       <c r="D17" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H17)&lt;&gt;0,'Sprint 1 - Planification'!H17,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E17" s="110"/>
       <c r="F17" s="111"/>
@@ -9738,17 +10097,17 @@
       <c r="P17" s="8"/>
     </row>
     <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B18" s="52" t="str">
+      <c r="B18" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B18)&lt;&gt;0,'Sprint 1 - Planification'!B18,"")</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="C18" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C18)&lt;&gt;0,'Sprint 1 - Planification'!C18,"")</f>
-        <v/>
+        <v>Faire la page liste des pièces/items</v>
       </c>
       <c r="D18" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H18)&lt;&gt;0,'Sprint 1 - Planification'!H18,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E18" s="116"/>
       <c r="F18" s="114"/>
@@ -9768,17 +10127,17 @@
       <c r="P18" s="8"/>
     </row>
     <row r="19" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B19" s="49" t="str">
+      <c r="B19" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B19)&lt;&gt;0,'Sprint 1 - Planification'!B19,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="C19" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C19)&lt;&gt;0,'Sprint 1 - Planification'!C19,"")</f>
-        <v/>
+        <v>Faire la page détails d'une pièce</v>
       </c>
       <c r="D19" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H19)&lt;&gt;0,'Sprint 1 - Planification'!H19,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E19" s="110"/>
       <c r="F19" s="111"/>
@@ -9798,17 +10157,17 @@
       <c r="P19" s="8"/>
     </row>
     <row r="20" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B20" s="52" t="str">
+      <c r="B20" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B20)&lt;&gt;0,'Sprint 1 - Planification'!B20,"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C20" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C20)&lt;&gt;0,'Sprint 1 - Planification'!C20,"")</f>
-        <v/>
+        <v>Faire la page pour les stats de base d'un item</v>
       </c>
       <c r="D20" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H20)&lt;&gt;0,'Sprint 1 - Planification'!H20,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E20" s="116"/>
       <c r="F20" s="114"/>
@@ -9828,17 +10187,17 @@
       <c r="P20" s="8"/>
     </row>
     <row r="21" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B21" s="49" t="str">
+      <c r="B21" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B21)&lt;&gt;0,'Sprint 1 - Planification'!B21,"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C21" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C21)&lt;&gt;0,'Sprint 1 - Planification'!C21,"")</f>
-        <v/>
+        <v>Faire le layout par défaut pour Nuxt</v>
       </c>
       <c r="D21" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H21)&lt;&gt;0,'Sprint 1 - Planification'!H21,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E21" s="110"/>
       <c r="F21" s="111"/>
@@ -9858,17 +10217,17 @@
       <c r="P21" s="8"/>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B22" s="52" t="str">
+      <c r="B22" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B22)&lt;&gt;0,'Sprint 1 - Planification'!B22,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C22" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C22)&lt;&gt;0,'Sprint 1 - Planification'!C22,"")</f>
-        <v/>
+        <v>Exporter les vraies données du jeu et importer dans bd</v>
       </c>
       <c r="D22" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H22)&lt;&gt;0,'Sprint 1 - Planification'!H22,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E22" s="113"/>
       <c r="F22" s="114"/>
@@ -9888,17 +10247,17 @@
       <c r="P22" s="8"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B23" s="49" t="str">
+      <c r="B23" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B23)&lt;&gt;0,'Sprint 1 - Planification'!B23,"")</f>
-        <v/>
+        <v>16</v>
       </c>
       <c r="C23" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C23)&lt;&gt;0,'Sprint 1 - Planification'!C23,"")</f>
-        <v/>
+        <v>Rédiger le rapport de projet</v>
       </c>
       <c r="D23" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H23)&lt;&gt;0,'Sprint 1 - Planification'!H23,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E23" s="110"/>
       <c r="F23" s="111"/>
@@ -9918,17 +10277,17 @@
       <c r="P23" s="8"/>
     </row>
     <row r="24" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B24" s="52" t="str">
+      <c r="B24" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B24)&lt;&gt;0,'Sprint 1 - Planification'!B24,"")</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="C24" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C24)&lt;&gt;0,'Sprint 1 - Planification'!C24,"")</f>
-        <v/>
+        <v>Rédiger le fichier Lisez_moi.txt</v>
       </c>
       <c r="D24" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H24)&lt;&gt;0,'Sprint 1 - Planification'!H24,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E24" s="116"/>
       <c r="F24" s="114"/>
@@ -9948,17 +10307,17 @@
       <c r="P24" s="8"/>
     </row>
     <row r="25" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B25" s="49" t="str">
+      <c r="B25" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B25)&lt;&gt;0,'Sprint 1 - Planification'!B25,"")</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C25" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C25)&lt;&gt;0,'Sprint 1 - Planification'!C25,"")</f>
-        <v/>
+        <v>Réaliser le site web de présentation</v>
       </c>
       <c r="D25" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H25)&lt;&gt;0,'Sprint 1 - Planification'!H25,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E25" s="110"/>
       <c r="F25" s="111"/>
@@ -9978,17 +10337,17 @@
       <c r="P25" s="8"/>
     </row>
     <row r="26" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="52" t="str">
+      <c r="B26" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C26" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>Réaliser la vidéo de présentation</v>
       </c>
       <c r="D26" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E26" s="116"/>
       <c r="F26" s="114"/>
@@ -10008,17 +10367,17 @@
       <c r="P26" s="8"/>
     </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="49" t="str">
+      <c r="B27" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C27" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>Faire une page détails fabriquant</v>
       </c>
       <c r="D27" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E27" s="110"/>
       <c r="F27" s="111"/>
@@ -10038,17 +10397,17 @@
       <c r="P27" s="8"/>
     </row>
     <row r="28" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="52" t="str">
+      <c r="B28" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C28" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>Ajouter les boucliers comme type d'item</v>
       </c>
       <c r="D28" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E28" s="113"/>
       <c r="F28" s="114"/>
@@ -10068,17 +10427,17 @@
       <c r="P28" s="8"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="49" t="str">
+      <c r="B29" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B29)&lt;&gt;0,'Sprint 1 - Planification'!B29,"")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="C29" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C29)&lt;&gt;0,'Sprint 1 - Planification'!C29,"")</f>
-        <v/>
+        <v>ajouter les grenades comme type d'item</v>
       </c>
       <c r="D29" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H29)&lt;&gt;0,'Sprint 1 - Planification'!H29,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E29" s="110"/>
       <c r="F29" s="111"/>
@@ -10098,17 +10457,17 @@
       <c r="P29" s="8"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="52" t="str">
+      <c r="B30" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B30)&lt;&gt;0,'Sprint 1 - Planification'!B30,"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="C30" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C30)&lt;&gt;0,'Sprint 1 - Planification'!C30,"")</f>
-        <v/>
+        <v>Ajouter les reliques comme type d'item</v>
       </c>
       <c r="D30" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H30)&lt;&gt;0,'Sprint 1 - Planification'!H30,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E30" s="116"/>
       <c r="F30" s="114"/>
@@ -10128,17 +10487,17 @@
       <c r="P30" s="8"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="49" t="str">
+      <c r="B31" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B31)&lt;&gt;0,'Sprint 1 - Planification'!B31,"")</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="C31" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C31)&lt;&gt;0,'Sprint 1 - Planification'!C31,"")</f>
-        <v/>
+        <v>Ajouter les class mods comme type d'item</v>
       </c>
       <c r="D31" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H31)&lt;&gt;0,'Sprint 1 - Planification'!H31,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E31" s="110"/>
       <c r="F31" s="111"/>
@@ -10158,17 +10517,17 @@
       <c r="P31" s="8"/>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="52" t="str">
+      <c r="B32" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B32)&lt;&gt;0,'Sprint 1 - Planification'!B32,"")</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="C32" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C32)&lt;&gt;0,'Sprint 1 - Planification'!C32,"")</f>
-        <v/>
+        <v>Ajouter les items uniques</v>
       </c>
       <c r="D32" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H32)&lt;&gt;0,'Sprint 1 - Planification'!H32,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E32" s="116"/>
       <c r="F32" s="114"/>
@@ -10696,7 +11055,7 @@
     <row r="2" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="122" t="str">
         <f>'Sprint 1 - Planification'!B2:H2</f>
-        <v>Nom du projet super cool que vous faites!</v>
+        <v>Calculatrice de statistiques d'items pour le jeu Borderlands 2</v>
       </c>
       <c r="C2" s="122"/>
       <c r="D2" s="122"/>
@@ -10708,7 +11067,7 @@
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="32"/>
@@ -10730,7 +11089,7 @@
     </row>
     <row r="5" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -10740,7 +11099,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="63" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 8 champs à remplir!</v>
+        <v>Attention, il reste 28 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -10749,23 +11108,23 @@
         <v>0</v>
       </c>
       <c r="C7" s="128" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="126" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="124" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="125"/>
       <c r="G7" s="130" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="134" t="s">
         <v>23</v>
-      </c>
-      <c r="I7" s="134" t="s">
-        <v>24</v>
       </c>
       <c r="M7" s="7"/>
     </row>
@@ -10774,10 +11133,10 @@
       <c r="C8" s="129"/>
       <c r="D8" s="127"/>
       <c r="E8" s="64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="131"/>
       <c r="H8" s="133"/>
@@ -11000,17 +11359,17 @@
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="str">
+      <c r="B13" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B12)&lt;&gt;0,'Sprint 1 - Planification'!B12,"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="C13" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C12)&lt;&gt;0,'Sprint 1 - Planification'!C12,"")</f>
-        <v/>
+        <v>Configurer le serveur</v>
       </c>
       <c r="D13" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H12)&lt;&gt;0,'Sprint 1 - Planification'!H12,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E13" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E12),"",'Sprint 1 - Bilan'!E12)</f>
@@ -11025,11 +11384,11 @@
       <c r="I13" s="115"/>
       <c r="M13" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11037,11 +11396,11 @@
       </c>
       <c r="P13" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="8"/>
       <c r="U13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V13" s="62">
         <f>V11</f>
@@ -11053,17 +11412,17 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="49" t="str">
+      <c r="B14" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B13)&lt;&gt;0,'Sprint 1 - Planification'!B13,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="C14" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C13)&lt;&gt;0,'Sprint 1 - Planification'!C13,"")</f>
-        <v/>
+        <v>Mettre en place l'API</v>
       </c>
       <c r="D14" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E14" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E13),"",'Sprint 1 - Bilan'!E13)</f>
@@ -11078,11 +11437,11 @@
       <c r="I14" s="112"/>
       <c r="M14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11090,11 +11449,11 @@
       </c>
       <c r="P14" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14" s="8"/>
       <c r="U14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V14" s="4">
         <f>V12</f>
@@ -11106,17 +11465,17 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="52" t="str">
+      <c r="B15" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B14)&lt;&gt;0,'Sprint 1 - Planification'!B14,"")</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="C15" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C14)&lt;&gt;0,'Sprint 1 - Planification'!C14,"")</f>
-        <v/>
+        <v>Configurer Nuxt</v>
       </c>
       <c r="D15" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E15" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E14),"",'Sprint 1 - Bilan'!E14)</f>
@@ -11131,11 +11490,11 @@
       <c r="I15" s="115"/>
       <c r="M15" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11143,7 +11502,7 @@
       </c>
       <c r="P15" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
@@ -11156,17 +11515,17 @@
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="49" t="str">
+      <c r="B16" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B15)&lt;&gt;0,'Sprint 1 - Planification'!B15,"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="C16" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C15)&lt;&gt;0,'Sprint 1 - Planification'!C15,"")</f>
-        <v/>
+        <v>Écrire un script pour populer la base de données</v>
       </c>
       <c r="D16" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E16" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E15),"",'Sprint 1 - Bilan'!E15)</f>
@@ -11181,11 +11540,11 @@
       <c r="I16" s="112"/>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11193,30 +11552,30 @@
       </c>
       <c r="P16" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche est en retard!",CONCATENATE(V16," tâches sont en retard!")))</f>
-        <v>4 tâches sont en retard!</v>
+        <v>14 tâches sont en retard!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="str">
+      <c r="B17" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B16)&lt;&gt;0,'Sprint 1 - Planification'!B16,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="C17" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C16)&lt;&gt;0,'Sprint 1 - Planification'!C16,"")</f>
-        <v/>
+        <v>Calcul des statistiques</v>
       </c>
       <c r="D17" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E17" s="72" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E16),"",'Sprint 1 - Bilan'!E16)</f>
@@ -11231,11 +11590,11 @@
       <c r="I17" s="115"/>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11243,22 +11602,22 @@
       </c>
       <c r="P17" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="49" t="str">
+      <c r="B18" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B17)&lt;&gt;0,'Sprint 1 - Planification'!B17,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="C18" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C17)&lt;&gt;0,'Sprint 1 - Planification'!C17,"")</f>
-        <v/>
+        <v>Faire la page sélection des pièces</v>
       </c>
       <c r="D18" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H17)&lt;&gt;0,'Sprint 1 - Planification'!H17,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E18" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E17),"",'Sprint 1 - Bilan'!E17)</f>
@@ -11273,11 +11632,11 @@
       <c r="I18" s="112"/>
       <c r="M18" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11285,22 +11644,22 @@
       </c>
       <c r="P18" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="8"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="52" t="str">
+      <c r="B19" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B18)&lt;&gt;0,'Sprint 1 - Planification'!B18,"")</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="C19" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C18)&lt;&gt;0,'Sprint 1 - Planification'!C18,"")</f>
-        <v/>
+        <v>Faire la page liste des pièces/items</v>
       </c>
       <c r="D19" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H18)&lt;&gt;0,'Sprint 1 - Planification'!H18,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E19" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E18),"",'Sprint 1 - Bilan'!E18)</f>
@@ -11316,11 +11675,11 @@
       <c r="K19" s="9"/>
       <c r="M19" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11328,22 +11687,22 @@
       </c>
       <c r="P19" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="8"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="49" t="str">
+      <c r="B20" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B19)&lt;&gt;0,'Sprint 1 - Planification'!B19,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="C20" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C19)&lt;&gt;0,'Sprint 1 - Planification'!C19,"")</f>
-        <v/>
+        <v>Faire la page détails d'une pièce</v>
       </c>
       <c r="D20" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H19)&lt;&gt;0,'Sprint 1 - Planification'!H19,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E20" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E19),"",'Sprint 1 - Bilan'!E19)</f>
@@ -11358,11 +11717,11 @@
       <c r="I20" s="112"/>
       <c r="M20" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11370,22 +11729,22 @@
       </c>
       <c r="P20" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="52" t="str">
+      <c r="B21" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B20)&lt;&gt;0,'Sprint 1 - Planification'!B20,"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C21" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C20)&lt;&gt;0,'Sprint 1 - Planification'!C20,"")</f>
-        <v/>
+        <v>Faire la page pour les stats de base d'un item</v>
       </c>
       <c r="D21" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H20)&lt;&gt;0,'Sprint 1 - Planification'!H20,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E21" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E20),"",'Sprint 1 - Bilan'!E20)</f>
@@ -11400,11 +11759,11 @@
       <c r="I21" s="115"/>
       <c r="M21" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11412,22 +11771,22 @@
       </c>
       <c r="P21" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="str">
+      <c r="B22" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B21)&lt;&gt;0,'Sprint 1 - Planification'!B21,"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C22" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C21)&lt;&gt;0,'Sprint 1 - Planification'!C21,"")</f>
-        <v/>
+        <v>Faire le layout par défaut pour Nuxt</v>
       </c>
       <c r="D22" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H21)&lt;&gt;0,'Sprint 1 - Planification'!H21,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E22" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E21),"",'Sprint 1 - Bilan'!E21)</f>
@@ -11442,11 +11801,11 @@
       <c r="I22" s="112"/>
       <c r="M22" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11454,22 +11813,22 @@
       </c>
       <c r="P22" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" s="8"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="str">
+      <c r="B23" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B22)&lt;&gt;0,'Sprint 1 - Planification'!B22,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C23" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C22)&lt;&gt;0,'Sprint 1 - Planification'!C22,"")</f>
-        <v/>
+        <v>Exporter les vraies données du jeu et importer dans bd</v>
       </c>
       <c r="D23" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H22)&lt;&gt;0,'Sprint 1 - Planification'!H22,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E23" s="72" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E22),"",'Sprint 1 - Bilan'!E22)</f>
@@ -11501,17 +11860,17 @@
       <c r="R23" s="8"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="49" t="str">
+      <c r="B24" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B23)&lt;&gt;0,'Sprint 1 - Planification'!B23,"")</f>
-        <v/>
+        <v>16</v>
       </c>
       <c r="C24" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C23)&lt;&gt;0,'Sprint 1 - Planification'!C23,"")</f>
-        <v/>
+        <v>Rédiger le rapport de projet</v>
       </c>
       <c r="D24" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H23)&lt;&gt;0,'Sprint 1 - Planification'!H23,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E24" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E23),"",'Sprint 1 - Bilan'!E23)</f>
@@ -11543,17 +11902,17 @@
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="52" t="str">
+      <c r="B25" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B24)&lt;&gt;0,'Sprint 1 - Planification'!B24,"")</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="C25" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C24)&lt;&gt;0,'Sprint 1 - Planification'!C24,"")</f>
-        <v/>
+        <v>Rédiger le fichier Lisez_moi.txt</v>
       </c>
       <c r="D25" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H24)&lt;&gt;0,'Sprint 1 - Planification'!H24,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E25" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E24),"",'Sprint 1 - Bilan'!E24)</f>
@@ -11585,17 +11944,17 @@
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="49" t="str">
+      <c r="B26" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B25)&lt;&gt;0,'Sprint 1 - Planification'!B25,"")</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C26" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C25)&lt;&gt;0,'Sprint 1 - Planification'!C25,"")</f>
-        <v/>
+        <v>Réaliser le site web de présentation</v>
       </c>
       <c r="D26" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H25)&lt;&gt;0,'Sprint 1 - Planification'!H25,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E26" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E25),"",'Sprint 1 - Bilan'!E25)</f>
@@ -11627,17 +11986,17 @@
       <c r="R26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="52" t="str">
+      <c r="B27" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C27" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>Réaliser la vidéo de présentation</v>
       </c>
       <c r="D27" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E27" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E26),"",'Sprint 1 - Bilan'!E26)</f>
@@ -11669,17 +12028,17 @@
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="49" t="str">
+      <c r="B28" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C28" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>Faire une page détails fabriquant</v>
       </c>
       <c r="D28" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E28" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E27),"",'Sprint 1 - Bilan'!E27)</f>
@@ -11711,17 +12070,17 @@
       <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="52" t="str">
+      <c r="B29" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C29" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>Ajouter les boucliers comme type d'item</v>
       </c>
       <c r="D29" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E29" s="72" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E28),"",'Sprint 1 - Bilan'!E28)</f>
@@ -11753,17 +12112,17 @@
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="49" t="str">
+      <c r="B30" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B29)&lt;&gt;0,'Sprint 1 - Planification'!B29,"")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="C30" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C29)&lt;&gt;0,'Sprint 1 - Planification'!C29,"")</f>
-        <v/>
+        <v>ajouter les grenades comme type d'item</v>
       </c>
       <c r="D30" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H29)&lt;&gt;0,'Sprint 1 - Planification'!H29,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E30" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E29),"",'Sprint 1 - Bilan'!E29)</f>
@@ -11795,17 +12154,17 @@
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="52" t="str">
+      <c r="B31" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B30)&lt;&gt;0,'Sprint 1 - Planification'!B30,"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="C31" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C30)&lt;&gt;0,'Sprint 1 - Planification'!C30,"")</f>
-        <v/>
+        <v>Ajouter les reliques comme type d'item</v>
       </c>
       <c r="D31" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H30)&lt;&gt;0,'Sprint 1 - Planification'!H30,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E31" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E30),"",'Sprint 1 - Bilan'!E30)</f>
@@ -11837,17 +12196,17 @@
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="str">
+      <c r="B32" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B31)&lt;&gt;0,'Sprint 1 - Planification'!B31,"")</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="C32" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C31)&lt;&gt;0,'Sprint 1 - Planification'!C31,"")</f>
-        <v/>
+        <v>Ajouter les class mods comme type d'item</v>
       </c>
       <c r="D32" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H31)&lt;&gt;0,'Sprint 1 - Planification'!H31,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E32" s="71" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E31),"",'Sprint 1 - Bilan'!E31)</f>
@@ -11879,17 +12238,17 @@
       <c r="R32" s="8"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="52" t="str">
+      <c r="B33" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B32)&lt;&gt;0,'Sprint 1 - Planification'!B32,"")</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="C33" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C32)&lt;&gt;0,'Sprint 1 - Planification'!C32,"")</f>
-        <v/>
+        <v>Ajouter les items uniques</v>
       </c>
       <c r="D33" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H32)&lt;&gt;0,'Sprint 1 - Planification'!H32,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E33" s="73" t="str">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E32),"",'Sprint 1 - Bilan'!E32)</f>
@@ -12343,11 +12702,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -12355,21 +12714,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>8 champs</v>
+        <v>28 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -12566,7 +12925,7 @@
     <row r="2" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="122" t="str">
         <f>'Sprint 1 - Planification'!B2:H2</f>
-        <v>Nom du projet super cool que vous faites!</v>
+        <v>Calculatrice de statistiques d'items pour le jeu Borderlands 2</v>
       </c>
       <c r="C2" s="122"/>
       <c r="D2" s="122"/>
@@ -12578,7 +12937,7 @@
     </row>
     <row r="3" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="32"/>
@@ -12600,7 +12959,7 @@
     </row>
     <row r="5" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="34"/>
@@ -12610,7 +12969,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="63" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 8 champs à remplir!</v>
+        <v>Attention, il reste 50 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -12619,23 +12978,23 @@
         <v>0</v>
       </c>
       <c r="C7" s="128" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" s="126" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="124" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="125"/>
       <c r="G7" s="130" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H7" s="132" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="134" t="s">
         <v>23</v>
-      </c>
-      <c r="I7" s="134" t="s">
-        <v>24</v>
       </c>
       <c r="M7" s="7"/>
     </row>
@@ -12644,10 +13003,10 @@
       <c r="C8" s="129"/>
       <c r="D8" s="127"/>
       <c r="E8" s="64" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" s="64" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="131"/>
       <c r="H8" s="133"/>
@@ -12870,17 +13229,17 @@
       </c>
     </row>
     <row r="13" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B13" s="52" t="str">
+      <c r="B13" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B12)&lt;&gt;0,'Sprint 1 - Planification'!B12,"")</f>
-        <v/>
+        <v>5</v>
       </c>
       <c r="C13" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C12)&lt;&gt;0,'Sprint 1 - Planification'!C12,"")</f>
-        <v/>
+        <v>Configurer le serveur</v>
       </c>
       <c r="D13" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H12)&lt;&gt;0,'Sprint 1 - Planification'!H12,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E13" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E13)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G13))</f>
@@ -12895,11 +13254,11 @@
       <c r="I13" s="115"/>
       <c r="M13" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N13" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12907,11 +13266,11 @@
       </c>
       <c r="P13" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R13" s="8"/>
       <c r="U13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="V13" s="62">
         <f>V11</f>
@@ -12923,17 +13282,17 @@
       </c>
     </row>
     <row r="14" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B14" s="49" t="str">
+      <c r="B14" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B13)&lt;&gt;0,'Sprint 1 - Planification'!B13,"")</f>
-        <v/>
+        <v>6</v>
       </c>
       <c r="C14" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C13)&lt;&gt;0,'Sprint 1 - Planification'!C13,"")</f>
-        <v/>
+        <v>Mettre en place l'API</v>
       </c>
       <c r="D14" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H13)&lt;&gt;0,'Sprint 1 - Planification'!H13,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E14" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E14)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G14))</f>
@@ -12948,11 +13307,11 @@
       <c r="I14" s="112"/>
       <c r="M14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="3" t="b">
         <f t="shared" si="2"/>
@@ -12960,11 +13319,11 @@
       </c>
       <c r="P14" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R14" s="8"/>
       <c r="U14" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="V14" s="4">
         <f>V12</f>
@@ -12976,17 +13335,17 @@
       </c>
     </row>
     <row r="15" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B15" s="52" t="str">
+      <c r="B15" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B14)&lt;&gt;0,'Sprint 1 - Planification'!B14,"")</f>
-        <v/>
+        <v>7</v>
       </c>
       <c r="C15" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C14)&lt;&gt;0,'Sprint 1 - Planification'!C14,"")</f>
-        <v/>
+        <v>Configurer Nuxt</v>
       </c>
       <c r="D15" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H14)&lt;&gt;0,'Sprint 1 - Planification'!H14,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E15" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E15)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G15))</f>
@@ -13001,11 +13360,11 @@
       <c r="I15" s="115"/>
       <c r="M15" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O15" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13013,7 +13372,7 @@
       </c>
       <c r="P15" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R15" s="8"/>
       <c r="W15" s="4" t="str">
@@ -13026,17 +13385,17 @@
       </c>
     </row>
     <row r="16" spans="2:25" x14ac:dyDescent="0.25">
-      <c r="B16" s="49" t="str">
+      <c r="B16" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B15)&lt;&gt;0,'Sprint 1 - Planification'!B15,"")</f>
-        <v/>
+        <v>8</v>
       </c>
       <c r="C16" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C15)&lt;&gt;0,'Sprint 1 - Planification'!C15,"")</f>
-        <v/>
+        <v>Écrire un script pour populer la base de données</v>
       </c>
       <c r="D16" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H15)&lt;&gt;0,'Sprint 1 - Planification'!H15,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E16" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E16)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G16)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E16)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G16))</f>
@@ -13051,11 +13410,11 @@
       <c r="I16" s="112"/>
       <c r="M16" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13063,30 +13422,30 @@
       </c>
       <c r="P16" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>4 tâches n'ont pas été terminé!</v>
+        <v>25 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="str">
+      <c r="B17" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B16)&lt;&gt;0,'Sprint 1 - Planification'!B16,"")</f>
-        <v/>
+        <v>9</v>
       </c>
       <c r="C17" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C16)&lt;&gt;0,'Sprint 1 - Planification'!C16,"")</f>
-        <v/>
+        <v>Calcul des statistiques</v>
       </c>
       <c r="D17" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H16)&lt;&gt;0,'Sprint 1 - Planification'!H16,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E17" s="72" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E17)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G17))</f>
@@ -13101,11 +13460,11 @@
       <c r="I17" s="115"/>
       <c r="M17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O17" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13113,22 +13472,22 @@
       </c>
       <c r="P17" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17" s="8"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B18" s="49" t="str">
+      <c r="B18" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B17)&lt;&gt;0,'Sprint 1 - Planification'!B17,"")</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="C18" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C17)&lt;&gt;0,'Sprint 1 - Planification'!C17,"")</f>
-        <v/>
+        <v>Faire la page sélection des pièces</v>
       </c>
       <c r="D18" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H17)&lt;&gt;0,'Sprint 1 - Planification'!H17,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E18" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E18)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G18)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E18)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G18))</f>
@@ -13143,11 +13502,11 @@
       <c r="I18" s="112"/>
       <c r="M18" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13155,22 +13514,22 @@
       </c>
       <c r="P18" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R18" s="8"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B19" s="52" t="str">
+      <c r="B19" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B18)&lt;&gt;0,'Sprint 1 - Planification'!B18,"")</f>
-        <v/>
+        <v>11</v>
       </c>
       <c r="C19" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C18)&lt;&gt;0,'Sprint 1 - Planification'!C18,"")</f>
-        <v/>
+        <v>Faire la page liste des pièces/items</v>
       </c>
       <c r="D19" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H18)&lt;&gt;0,'Sprint 1 - Planification'!H18,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E19" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E19)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G19)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E19)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G19))</f>
@@ -13185,11 +13544,11 @@
       <c r="I19" s="115"/>
       <c r="M19" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13197,22 +13556,22 @@
       </c>
       <c r="P19" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R19" s="8"/>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B20" s="49" t="str">
+      <c r="B20" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B19)&lt;&gt;0,'Sprint 1 - Planification'!B19,"")</f>
-        <v/>
+        <v>12</v>
       </c>
       <c r="C20" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C19)&lt;&gt;0,'Sprint 1 - Planification'!C19,"")</f>
-        <v/>
+        <v>Faire la page détails d'une pièce</v>
       </c>
       <c r="D20" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H19)&lt;&gt;0,'Sprint 1 - Planification'!H19,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E20" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E20)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G20)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E20)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G20))</f>
@@ -13227,11 +13586,11 @@
       <c r="I20" s="112"/>
       <c r="M20" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13239,22 +13598,22 @@
       </c>
       <c r="P20" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R20" s="8"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="52" t="str">
+      <c r="B21" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B20)&lt;&gt;0,'Sprint 1 - Planification'!B20,"")</f>
-        <v/>
+        <v>13</v>
       </c>
       <c r="C21" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C20)&lt;&gt;0,'Sprint 1 - Planification'!C20,"")</f>
-        <v/>
+        <v>Faire la page pour les stats de base d'un item</v>
       </c>
       <c r="D21" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H20)&lt;&gt;0,'Sprint 1 - Planification'!H20,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E21" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E21)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G21)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E21)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G21))</f>
@@ -13269,11 +13628,11 @@
       <c r="I21" s="115"/>
       <c r="M21" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O21" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13281,22 +13640,22 @@
       </c>
       <c r="P21" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R21" s="8"/>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="str">
+      <c r="B22" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B21)&lt;&gt;0,'Sprint 1 - Planification'!B21,"")</f>
-        <v/>
+        <v>14</v>
       </c>
       <c r="C22" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C21)&lt;&gt;0,'Sprint 1 - Planification'!C21,"")</f>
-        <v/>
+        <v>Faire le layout par défaut pour Nuxt</v>
       </c>
       <c r="D22" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H21)&lt;&gt;0,'Sprint 1 - Planification'!H21,"")</f>
-        <v/>
+        <v>Sprint 2</v>
       </c>
       <c r="E22" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E22)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G22)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E22)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G22))</f>
@@ -13311,11 +13670,11 @@
       <c r="I22" s="112"/>
       <c r="M22" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13323,22 +13682,22 @@
       </c>
       <c r="P22" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" s="8"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B23" s="52" t="str">
+      <c r="B23" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B22)&lt;&gt;0,'Sprint 1 - Planification'!B22,"")</f>
-        <v/>
+        <v>15</v>
       </c>
       <c r="C23" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C22)&lt;&gt;0,'Sprint 1 - Planification'!C22,"")</f>
-        <v/>
+        <v>Exporter les vraies données du jeu et importer dans bd</v>
       </c>
       <c r="D23" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H22)&lt;&gt;0,'Sprint 1 - Planification'!H22,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E23" s="72" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E23)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G23)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E23)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G23))</f>
@@ -13353,11 +13712,11 @@
       <c r="I23" s="115"/>
       <c r="M23" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O23" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13365,22 +13724,22 @@
       </c>
       <c r="P23" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R23" s="8"/>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B24" s="49" t="str">
+      <c r="B24" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B23)&lt;&gt;0,'Sprint 1 - Planification'!B23,"")</f>
-        <v/>
+        <v>16</v>
       </c>
       <c r="C24" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C23)&lt;&gt;0,'Sprint 1 - Planification'!C23,"")</f>
-        <v/>
+        <v>Rédiger le rapport de projet</v>
       </c>
       <c r="D24" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H23)&lt;&gt;0,'Sprint 1 - Planification'!H23,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E24" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E24)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G24)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E24)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G24))</f>
@@ -13395,11 +13754,11 @@
       <c r="I24" s="112"/>
       <c r="M24" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O24" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13407,22 +13766,22 @@
       </c>
       <c r="P24" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R24" s="8"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B25" s="52" t="str">
+      <c r="B25" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B24)&lt;&gt;0,'Sprint 1 - Planification'!B24,"")</f>
-        <v/>
+        <v>17</v>
       </c>
       <c r="C25" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C24)&lt;&gt;0,'Sprint 1 - Planification'!C24,"")</f>
-        <v/>
+        <v>Rédiger le fichier Lisez_moi.txt</v>
       </c>
       <c r="D25" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H24)&lt;&gt;0,'Sprint 1 - Planification'!H24,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E25" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E25)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G25)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E25)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G25))</f>
@@ -13437,11 +13796,11 @@
       <c r="I25" s="115"/>
       <c r="M25" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13449,22 +13808,22 @@
       </c>
       <c r="P25" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R25" s="8"/>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B26" s="49" t="str">
+      <c r="B26" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B25)&lt;&gt;0,'Sprint 1 - Planification'!B25,"")</f>
-        <v/>
+        <v>18</v>
       </c>
       <c r="C26" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C25)&lt;&gt;0,'Sprint 1 - Planification'!C25,"")</f>
-        <v/>
+        <v>Réaliser le site web de présentation</v>
       </c>
       <c r="D26" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H25)&lt;&gt;0,'Sprint 1 - Planification'!H25,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E26" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E26)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G26)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E26)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G26))</f>
@@ -13479,11 +13838,11 @@
       <c r="I26" s="112"/>
       <c r="M26" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O26" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13491,22 +13850,22 @@
       </c>
       <c r="P26" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R26" s="8"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B27" s="52" t="str">
+      <c r="B27" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B26)&lt;&gt;0,'Sprint 1 - Planification'!B26,"")</f>
-        <v/>
+        <v>19</v>
       </c>
       <c r="C27" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C26)&lt;&gt;0,'Sprint 1 - Planification'!C26,"")</f>
-        <v/>
+        <v>Réaliser la vidéo de présentation</v>
       </c>
       <c r="D27" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H26)&lt;&gt;0,'Sprint 1 - Planification'!H26,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E27" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E27)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G27)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E27)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G27))</f>
@@ -13521,11 +13880,11 @@
       <c r="I27" s="115"/>
       <c r="M27" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O27" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13533,22 +13892,22 @@
       </c>
       <c r="P27" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R27" s="8"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B28" s="49" t="str">
+      <c r="B28" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B27)&lt;&gt;0,'Sprint 1 - Planification'!B27,"")</f>
-        <v/>
+        <v>20</v>
       </c>
       <c r="C28" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C27)&lt;&gt;0,'Sprint 1 - Planification'!C27,"")</f>
-        <v/>
+        <v>Faire une page détails fabriquant</v>
       </c>
       <c r="D28" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H27)&lt;&gt;0,'Sprint 1 - Planification'!H27,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E28" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E28)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G28)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E28)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G28))</f>
@@ -13563,11 +13922,11 @@
       <c r="I28" s="112"/>
       <c r="M28" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O28" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13575,22 +13934,22 @@
       </c>
       <c r="P28" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R28" s="8"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B29" s="52" t="str">
+      <c r="B29" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B28)&lt;&gt;0,'Sprint 1 - Planification'!B28,"")</f>
-        <v/>
+        <v>21</v>
       </c>
       <c r="C29" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C28)&lt;&gt;0,'Sprint 1 - Planification'!C28,"")</f>
-        <v/>
+        <v>Ajouter les boucliers comme type d'item</v>
       </c>
       <c r="D29" s="54" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H28)&lt;&gt;0,'Sprint 1 - Planification'!H28,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E29" s="72" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E29)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G29))</f>
@@ -13605,11 +13964,11 @@
       <c r="I29" s="115"/>
       <c r="M29" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O29" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13617,22 +13976,22 @@
       </c>
       <c r="P29" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R29" s="8"/>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B30" s="49" t="str">
+      <c r="B30" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B29)&lt;&gt;0,'Sprint 1 - Planification'!B29,"")</f>
-        <v/>
+        <v>22</v>
       </c>
       <c r="C30" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C29)&lt;&gt;0,'Sprint 1 - Planification'!C29,"")</f>
-        <v/>
+        <v>ajouter les grenades comme type d'item</v>
       </c>
       <c r="D30" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H29)&lt;&gt;0,'Sprint 1 - Planification'!H29,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E30" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E30)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G30)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E30)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G30))</f>
@@ -13647,11 +14006,11 @@
       <c r="I30" s="112"/>
       <c r="M30" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O30" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13659,22 +14018,22 @@
       </c>
       <c r="P30" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R30" s="8"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B31" s="52" t="str">
+      <c r="B31" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B30)&lt;&gt;0,'Sprint 1 - Planification'!B30,"")</f>
-        <v/>
+        <v>23</v>
       </c>
       <c r="C31" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C30)&lt;&gt;0,'Sprint 1 - Planification'!C30,"")</f>
-        <v/>
+        <v>Ajouter les reliques comme type d'item</v>
       </c>
       <c r="D31" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H30)&lt;&gt;0,'Sprint 1 - Planification'!H30,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E31" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E31)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G31)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E31)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G31))</f>
@@ -13689,11 +14048,11 @@
       <c r="I31" s="115"/>
       <c r="M31" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O31" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13701,22 +14060,22 @@
       </c>
       <c r="P31" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R31" s="8"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B32" s="49" t="str">
+      <c r="B32" s="49">
         <f>IF(LEN('Sprint 1 - Planification'!B31)&lt;&gt;0,'Sprint 1 - Planification'!B31,"")</f>
-        <v/>
+        <v>24</v>
       </c>
       <c r="C32" s="50" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C31)&lt;&gt;0,'Sprint 1 - Planification'!C31,"")</f>
-        <v/>
+        <v>Ajouter les class mods comme type d'item</v>
       </c>
       <c r="D32" s="51" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H31)&lt;&gt;0,'Sprint 1 - Planification'!H31,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E32" s="71" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E32)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G32)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E32)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G32))</f>
@@ -13731,11 +14090,11 @@
       <c r="I32" s="112"/>
       <c r="M32" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N32" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O32" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13743,22 +14102,22 @@
       </c>
       <c r="P32" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R32" s="8"/>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.25">
-      <c r="B33" s="52" t="str">
+      <c r="B33" s="52">
         <f>IF(LEN('Sprint 1 - Planification'!B32)&lt;&gt;0,'Sprint 1 - Planification'!B32,"")</f>
-        <v/>
+        <v>25</v>
       </c>
       <c r="C33" s="53" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!C32)&lt;&gt;0,'Sprint 1 - Planification'!C32,"")</f>
-        <v/>
+        <v>Ajouter les items uniques</v>
       </c>
       <c r="D33" s="55" t="str">
         <f>IF(LEN('Sprint 1 - Planification'!H32)&lt;&gt;0,'Sprint 1 - Planification'!H32,"")</f>
-        <v/>
+        <v>Sprint 3</v>
       </c>
       <c r="E33" s="73" t="str">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E33)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G33)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E33)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G33))</f>
@@ -13773,11 +14132,11 @@
       <c r="I33" s="115"/>
       <c r="M33" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N33" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O33" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13785,7 +14144,7 @@
       </c>
       <c r="P33" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R33" s="8"/>
     </row>
@@ -14212,11 +14571,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -14224,21 +14583,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>8</v>
+        <v>50</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>8 champs</v>
+        <v>50 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -14381,7 +14740,7 @@
     <row r="1" spans="2:25" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="106" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="106"/>
       <c r="D2" s="106"/>
@@ -14394,7 +14753,7 @@
     </row>
     <row r="3" spans="2:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C3" s="86"/>
       <c r="D3" s="86"/>
@@ -14410,7 +14769,7 @@
     </row>
     <row r="5" spans="2:25" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="85" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="87"/>
       <c r="D5" s="87"/>
@@ -14434,7 +14793,7 @@
         <v>3</v>
       </c>
       <c r="F7" s="92" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -14449,7 +14808,7 @@
     </row>
     <row r="8" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B8" s="89" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="93">
         <f>L8</f>
@@ -14457,15 +14816,15 @@
       </c>
       <c r="D8" s="94">
         <f>M8</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E8" s="95">
         <f>N8</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="F8" s="99">
         <f>O8</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -14475,15 +14834,15 @@
       </c>
       <c r="M8" s="1">
         <f>'Sprint 1 - Planification'!AJ18</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="N8" s="1">
         <f>'Sprint 1 - Planification'!AJ19</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="O8" s="1">
         <f>SUM(L8:N8)</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
@@ -14492,7 +14851,7 @@
     </row>
     <row r="9" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B9" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="96" t="str">
         <f t="shared" ref="C9:F10" si="0">DAY(L9)*24+HOUR(L9)&amp;"h"&amp;TEXT(MINUTE(L9),"00")</f>
@@ -14500,15 +14859,15 @@
       </c>
       <c r="D9" s="97" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>29h30</v>
       </c>
       <c r="E9" s="98" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>27h45</v>
       </c>
       <c r="F9" s="100" t="str">
         <f t="shared" si="0"/>
-        <v>12h30</v>
+        <v>69h45</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -14518,18 +14877,18 @@
       </c>
       <c r="M9" s="1">
         <f>'Sprint 1 - Planification'!AD18</f>
-        <v>0</v>
+        <v>1.2291666666666663</v>
       </c>
       <c r="N9" s="1">
         <f>'Sprint 1 - Planification'!AD19</f>
-        <v>0</v>
+        <v>1.1562500000000004</v>
       </c>
       <c r="O9" s="1">
         <f>SUM(L9:N9)</f>
-        <v>0.5208333333333337</v>
+        <v>2.9062500000000004</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" ref="Q9:S10" si="1">DAY(L9)*24+HOUR(L9)+MINUTE(L9)/60</f>
@@ -14537,30 +14896,30 @@
       </c>
       <c r="R9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.5</v>
       </c>
       <c r="S9" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27.75</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="V9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Essentielle")</f>
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="X9" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="Y9" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,1)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B10" s="89" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="93" t="str">
         <f t="shared" si="0"/>
@@ -14597,7 +14956,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="1"/>
@@ -14612,23 +14971,23 @@
         <v>0</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="V10" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!E8:E42,"Optionnelle")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="Y10" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,2)</f>
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="2:25" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="101" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="102">
         <f>L11</f>
@@ -14636,15 +14995,15 @@
       </c>
       <c r="D11" s="103">
         <f>M11</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E11" s="104">
         <f>N11</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="F11" s="105">
         <f>O11</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -14654,26 +15013,26 @@
       </c>
       <c r="M11" s="1">
         <f>'Sprint 2 - Bilan'!V16</f>
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="X11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Y11" s="2">
         <f>COUNTIF('Sprint 1 - Planification'!F8:F42,3)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:25" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
@@ -14827,7 +15186,7 @@
     <row r="1" spans="2:8" ht="7.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="136" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="136"/>
       <c r="D2" s="136"/>
@@ -14838,7 +15197,7 @@
     </row>
     <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="25"/>
       <c r="D3" s="79"/>
@@ -14858,7 +15217,7 @@
     </row>
     <row r="5" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="28"/>
       <c r="D5" s="81"/>
@@ -14871,7 +15230,7 @@
     <row r="7" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="83" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="82"/>
       <c r="E7" s="1"/>
@@ -14882,7 +15241,7 @@
     <row r="8" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B8" s="82"/>
       <c r="D8" s="82" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -14892,7 +15251,7 @@
     <row r="9" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="D9" s="82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -14910,7 +15269,7 @@
     <row r="11" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="83" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D11" s="82"/>
       <c r="E11" s="1"/>
@@ -14921,7 +15280,7 @@
     <row r="12" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="D12" s="82" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -14931,7 +15290,7 @@
     <row r="13" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="D13" s="82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -14941,7 +15300,7 @@
     <row r="14" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="D14" s="82" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -14951,7 +15310,7 @@
     <row r="15" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="D15" s="82" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -14961,7 +15320,7 @@
     <row r="16" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="D16" s="82" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -14971,7 +15330,7 @@
     <row r="17" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="D17" s="82" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -14981,7 +15340,7 @@
     <row r="18" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="D18" s="82" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -14990,7 +15349,7 @@
     </row>
     <row r="20" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="81"/>
@@ -15003,7 +15362,7 @@
     <row r="22" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
       <c r="C22" s="83" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" s="82"/>
       <c r="E22" s="1"/>
@@ -15014,7 +15373,7 @@
     <row r="23" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B23" s="82"/>
       <c r="D23" s="82" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -15024,7 +15383,7 @@
     <row r="24" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
       <c r="D24" s="82" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -15034,7 +15393,7 @@
     <row r="25" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="D25" s="82" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -15051,7 +15410,7 @@
     </row>
     <row r="28" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" s="28"/>
       <c r="D28" s="81"/>
@@ -15064,7 +15423,7 @@
     <row r="30" spans="2:8" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="83" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D30" s="82"/>
       <c r="E30" s="1"/>
@@ -15082,7 +15441,7 @@
     </row>
     <row r="33" spans="2:8" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="28"/>
       <c r="D33" s="81"/>
@@ -15095,7 +15454,7 @@
     <row r="35" spans="2:8" s="2" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="137" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="137"/>
       <c r="E35" s="137"/>

</xml_diff>

<commit_message>
finir document de conception
</commit_message>
<xml_diff>
--- a/doc/B65_-_Hiver_2019_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
+++ b/doc/B65_-_Hiver_2019_-_Outil_de_planification_et_de_suivi_de_projet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ecole\synthese\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B567E58E-80F3-4CB6-890E-C401E05EDDB0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985BE762-B30A-4DFC-A398-265E89F5A3A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="494" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="494" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1 - Planification" sheetId="1" r:id="rId1"/>
@@ -2829,13 +2829,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3248,7 +3248,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -7048,7 +7048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AJ90"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -9627,8 +9627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:W56"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9685,7 +9685,7 @@
       <c r="F5" s="34"/>
       <c r="G5" s="63" t="str">
         <f>IF(K44=0,CONCATENATE("Ce sprint totalise ", U14, " de travail réalisé. ",U15),CONCATENATE("Attention, il reste ",K45," à remplir!"))</f>
-        <v>Attention, il reste 8 champs à remplir!</v>
+        <v xml:space="preserve">Ce sprint totalise 12 heures de travail réalisé. </v>
       </c>
     </row>
     <row r="6" spans="2:23" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -9723,16 +9723,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H8)&lt;&gt;0,'Sprint 1 - Planification'!H8,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E8" s="107"/>
-      <c r="F8" s="108"/>
+      <c r="E8" s="107">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F8" s="108">
+        <v>1</v>
+      </c>
       <c r="G8" s="109"/>
       <c r="K8" s="3" t="b">
         <f>AND($D8="Sprint 1",ISBLANK(E8))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="3" t="b">
         <f>AND($D8="Sprint 1",ISBLANK(F8))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="3" t="b">
         <f>AND($D8="Sprint 1",NOT(ISBLANK($F8)),$F8&lt;100%,ISBLANK($G8))</f>
@@ -9743,15 +9747,15 @@
       </c>
       <c r="Q8" s="60">
         <f t="array" ref="Q8">SUM(($D$8:$D$42=$P8)*$E$8:$E$42)</f>
-        <v>0</v>
+        <v>0.49999999999999967</v>
       </c>
       <c r="R8" s="61">
         <f>Q8*24*60</f>
-        <v>0</v>
+        <v>719.99999999999955</v>
       </c>
       <c r="T8" s="9">
         <f>SUM(E8:E42)</f>
-        <v>0</v>
+        <v>0.49999999999999967</v>
       </c>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.25">
@@ -9767,16 +9771,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H9)&lt;&gt;0,'Sprint 1 - Planification'!H9,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
+      <c r="E9" s="110">
+        <v>0.25</v>
+      </c>
+      <c r="F9" s="111">
+        <v>1</v>
+      </c>
       <c r="G9" s="112"/>
       <c r="K9" s="3" t="b">
         <f t="shared" ref="K9:K42" si="0">AND($D9="Sprint 1",ISBLANK(E9))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" s="3" t="b">
         <f t="shared" ref="L9:L42" si="1">AND($D9="Sprint 1",ISBLANK(F9))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M9" s="3" t="b">
         <f t="shared" ref="M9:M42" si="2">AND($D9="Sprint 1",NOT(ISBLANK($F9)),$F9&lt;100%,ISBLANK($G9))</f>
@@ -9795,7 +9803,7 @@
       </c>
       <c r="T9" s="10">
         <f>T8</f>
-        <v>0</v>
+        <v>0.49999999999999967</v>
       </c>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.25">
@@ -9811,16 +9819,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H10)&lt;&gt;0,'Sprint 1 - Planification'!H10,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114"/>
+      <c r="E10" s="113">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="F10" s="114">
+        <v>1</v>
+      </c>
       <c r="G10" s="115"/>
       <c r="K10" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M10" s="3" t="b">
         <f t="shared" si="2"/>
@@ -9839,7 +9851,7 @@
       </c>
       <c r="T10" s="62">
         <f>DAY(T8)*24+HOUR(T8)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.25">
@@ -9855,16 +9867,20 @@
         <f>IF(LEN('Sprint 1 - Planification'!H11)&lt;&gt;0,'Sprint 1 - Planification'!H11,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E11" s="110"/>
-      <c r="F11" s="111"/>
+      <c r="E11" s="110">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F11" s="111">
+        <v>1</v>
+      </c>
       <c r="G11" s="112"/>
       <c r="K11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M11" s="3" t="b">
         <f t="shared" si="2"/>
@@ -9912,11 +9928,11 @@
       </c>
       <c r="T12" s="62">
         <f>T10</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="U12" s="4" t="str">
         <f>T12 &amp; " " &amp; S12 &amp; IF(T12 &gt; 1, "s", "")</f>
-        <v>0 heure</v>
+        <v>12 heures</v>
       </c>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.25">
@@ -9991,11 +10007,11 @@
       <c r="P14" s="8"/>
       <c r="U14" s="4" t="str">
         <f>IF(T12&gt;0,IF(T13&gt;0,U12&amp;" et "&amp;U13,U12),U13)</f>
-        <v>0 minute</v>
+        <v>12 heures</v>
       </c>
       <c r="W14" s="4" t="str">
         <f>T12&amp;"h"&amp;TEXT(T13,"00")</f>
-        <v>0h00</v>
+        <v>12h00</v>
       </c>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.25">
@@ -10029,11 +10045,11 @@
       <c r="P15" s="8"/>
       <c r="T15" s="4">
         <f t="array" ref="T15">SUM(($D$8:$D$42="Sprint 1")*($F$8:$F$42&lt;1))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="U15" s="4" t="str">
         <f>IF(T15=0,"",IF(T15=1,"Une tâche est en retard!",CONCATENATE(T15," tâches sont en retard!")))</f>
-        <v>4 tâches sont en retard!</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="2:23" x14ac:dyDescent="0.25">
@@ -10849,11 +10865,11 @@
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K43" s="3">
         <f>COUNTIF(K8:K42,TRUE)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L43" s="3">
         <f t="shared" ref="L43:M43" si="4">COUNTIF(L8:L42,TRUE)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M43" s="3">
         <f t="shared" si="4"/>
@@ -10864,14 +10880,14 @@
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K44" s="3">
         <f>SUM(K43:M43)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="P44" s="8"/>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="K45" s="3" t="str">
         <f>IF(K44=0, "aucun champ", IF(K44=1, "1 champ", K44 &amp; " champs"))</f>
-        <v>8 champs</v>
+        <v>aucun champ</v>
       </c>
       <c r="P45" s="8"/>
     </row>
@@ -11099,7 +11115,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="63" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 28 champs à remplir!</v>
+        <v>Attention, il reste 20 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -11156,24 +11172,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H8)&lt;&gt;0,'Sprint 1 - Planification'!H8,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E9" s="70" t="str">
+      <c r="E9" s="70">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E8),"",'Sprint 1 - Bilan'!E8)</f>
-        <v/>
-      </c>
-      <c r="F9" s="69" t="str">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="F9" s="69">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F8),"",'Sprint 1 - Bilan'!F8)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G9" s="107"/>
       <c r="H9" s="108"/>
       <c r="I9" s="109"/>
       <c r="M9" s="3" t="b">
         <f>OR(AND(NOT(P9),LEN($G9)=0),AND(LEN($H9)&gt;0,LEN($G9)=0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3" t="b">
         <f>AND(NOT($P9),LEN($H9)=0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="3" t="b">
         <f>AND($D9&lt;&gt;"Sprint 3",NOT(ISBLANK($H9)),$H9&lt;100%,ISBLANK($I9))</f>
@@ -11181,7 +11197,7 @@
       </c>
       <c r="P9" s="3" t="b">
         <f>IF(OR(LEN($D9)=0,$D9="Sprint 3"),TRUE,IF(COUNTA($F9)=0,IF(LEN($H9)=0,FALSE,$H9=100%),IF($F9=100%,TRUE,IF(LEN($H9)=0,FALSE,$H9=100%))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>1</v>
@@ -11212,24 +11228,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H9)&lt;&gt;0,'Sprint 1 - Planification'!H9,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E10" s="71" t="str">
+      <c r="E10" s="71">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E9),"",'Sprint 1 - Bilan'!E9)</f>
-        <v/>
-      </c>
-      <c r="F10" s="75" t="str">
+        <v>0.25</v>
+      </c>
+      <c r="F10" s="75">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F9),"",'Sprint 1 - Bilan'!F9)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G10" s="110"/>
       <c r="H10" s="111"/>
       <c r="I10" s="112"/>
       <c r="M10" s="3" t="b">
         <f t="shared" ref="M10:M43" si="0">OR(AND(NOT(P10),LEN($G10)=0),AND(LEN($H10)&gt;0,LEN($G10)=0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="3" t="b">
         <f t="shared" ref="N10:N43" si="1">AND(NOT(P10),LEN($H10)=0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="3" t="b">
         <f t="shared" ref="O10:O43" si="2">AND($D10&lt;&gt;"Sprint 3",NOT(ISBLANK($H10)),$H10&lt;100%,ISBLANK($I10))</f>
@@ -11237,7 +11253,7 @@
       </c>
       <c r="P10" s="3" t="b">
         <f t="shared" ref="P10:P43" si="3">IF(OR(LEN($D10)=0,$D10="Sprint 3"),TRUE,IF(COUNTA($F10)=0,IF(LEN($H10)=0,FALSE,$H10=100%),IF($F10=100%,TRUE,IF(LEN($H10)=0,FALSE,$H10=100%))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>2</v>
@@ -11268,24 +11284,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H10)&lt;&gt;0,'Sprint 1 - Planification'!H10,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E11" s="72" t="str">
+      <c r="E11" s="72">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E10),"",'Sprint 1 - Bilan'!E10)</f>
-        <v/>
-      </c>
-      <c r="F11" s="76" t="str">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="F11" s="76">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F10),"",'Sprint 1 - Bilan'!F10)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G11" s="113"/>
       <c r="H11" s="114"/>
       <c r="I11" s="115"/>
       <c r="M11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11293,7 +11309,7 @@
       </c>
       <c r="P11" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>3</v>
@@ -11324,24 +11340,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H11)&lt;&gt;0,'Sprint 1 - Planification'!H11,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E12" s="71" t="str">
+      <c r="E12" s="71">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!E11),"",'Sprint 1 - Bilan'!E11)</f>
-        <v/>
-      </c>
-      <c r="F12" s="75" t="str">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F12" s="75">
         <f>IF(ISBLANK('Sprint 1 - Bilan'!F11),"",'Sprint 1 - Bilan'!F11)</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G12" s="110"/>
       <c r="H12" s="111"/>
       <c r="I12" s="112"/>
       <c r="M12" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="3" t="b">
         <f t="shared" si="2"/>
@@ -11349,7 +11365,7 @@
       </c>
       <c r="P12" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
@@ -11557,11 +11573,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche est en retard!",CONCATENATE(V16," tâches sont en retard!")))</f>
-        <v>14 tâches sont en retard!</v>
+        <v>10 tâches sont en retard!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -12702,11 +12718,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -12714,21 +12730,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>28 champs</v>
+        <v>20 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -12969,7 +12985,7 @@
       <c r="H5" s="34"/>
       <c r="I5" s="63" t="str">
         <f>IF(M45=0,CONCATENATE("Ce sprint totalise ", W15, " de travail réalisé. ",W16),CONCATENATE("Attention, il reste ",M46," à remplir!"))</f>
-        <v>Attention, il reste 50 champs à remplir!</v>
+        <v>Attention, il reste 42 champs à remplir!</v>
       </c>
     </row>
     <row r="6" spans="2:25" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -13026,24 +13042,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H8)&lt;&gt;0,'Sprint 1 - Planification'!H8,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E9" s="70" t="str">
+      <c r="E9" s="70">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E9)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G9)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E9)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G9))</f>
-        <v/>
-      </c>
-      <c r="F9" s="69" t="str">
+        <v>1.0416666666666701E-2</v>
+      </c>
+      <c r="F9" s="69">
         <f>IF(LEN('Sprint 2 - Bilan'!$H9)&lt;&gt;0,'Sprint 2 - Bilan'!$H9,IF(LEN('Sprint 2 - Bilan'!$F9)=0,"",'Sprint 2 - Bilan'!$F9))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G9" s="107"/>
       <c r="H9" s="108"/>
       <c r="I9" s="109"/>
       <c r="M9" s="3" t="b">
         <f>OR(AND(NOT(P9),LEN($G9)=0),AND(LEN($H9)&gt;0,LEN($G9)=0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="3" t="b">
         <f>AND(NOT($P9),LEN($H9)=0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O9" s="3" t="b">
         <f>AND(LEN($H9)&gt;0,$H9&lt;100%,LEN($I9)=0)</f>
@@ -13051,7 +13067,7 @@
       </c>
       <c r="P9" s="3" t="b">
         <f>IF(LEN($C9)=0,TRUE,IF(LEN($F9)=0,IF(LEN($H9)=0,FALSE,$H9=100%),IF($F9=100%,TRUE,IF(LEN($H9)=0,FALSE,$H9=100%))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R9" s="4" t="s">
         <v>1</v>
@@ -13082,24 +13098,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H9)&lt;&gt;0,'Sprint 1 - Planification'!H9,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E10" s="71" t="str">
+      <c r="E10" s="71">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E10)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G10)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E10)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G10))</f>
-        <v/>
-      </c>
-      <c r="F10" s="75" t="str">
+        <v>0.25</v>
+      </c>
+      <c r="F10" s="75">
         <f>IF(LEN('Sprint 2 - Bilan'!$H10)&lt;&gt;0,'Sprint 2 - Bilan'!$H10,IF(LEN('Sprint 2 - Bilan'!$F10)=0,"",'Sprint 2 - Bilan'!$F10))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G10" s="110"/>
       <c r="H10" s="111"/>
       <c r="I10" s="112"/>
       <c r="M10" s="3" t="b">
         <f t="shared" ref="M10:M43" si="0">OR(AND(NOT(P10),LEN($G10)=0),AND(LEN($H10)&gt;0,LEN($G10)=0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10" s="3" t="b">
         <f t="shared" ref="N10:N43" si="1">AND(NOT($P10),LEN($H10)=0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="3" t="b">
         <f t="shared" ref="O10:O43" si="2">AND(LEN($H10)&gt;0,$H10&lt;100%,LEN($I10)=0)</f>
@@ -13107,7 +13123,7 @@
       </c>
       <c r="P10" s="3" t="b">
         <f t="shared" ref="P10:P43" si="3">IF(LEN($C10)=0,TRUE,IF(LEN($F10)=0,IF(LEN($H10)=0,FALSE,$H10=100%),IF($F10=100%,TRUE,IF(LEN($H10)=0,FALSE,$H10=100%))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R10" s="4" t="s">
         <v>2</v>
@@ -13138,24 +13154,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H10)&lt;&gt;0,'Sprint 1 - Planification'!H10,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E11" s="72" t="str">
+      <c r="E11" s="72">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E11)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G11)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E11)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G11))</f>
-        <v/>
-      </c>
-      <c r="F11" s="76" t="str">
+        <v>0.20833333333333301</v>
+      </c>
+      <c r="F11" s="76">
         <f>IF(LEN('Sprint 2 - Bilan'!$H11)&lt;&gt;0,'Sprint 2 - Bilan'!$H11,IF(LEN('Sprint 2 - Bilan'!$F11)=0,"",'Sprint 2 - Bilan'!$F11))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G11" s="113"/>
       <c r="H11" s="114"/>
       <c r="I11" s="115"/>
       <c r="M11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13163,7 +13179,7 @@
       </c>
       <c r="P11" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="4" t="s">
         <v>3</v>
@@ -13194,24 +13210,24 @@
         <f>IF(LEN('Sprint 1 - Planification'!H11)&lt;&gt;0,'Sprint 1 - Planification'!H11,"")</f>
         <v>Sprint 1</v>
       </c>
-      <c r="E12" s="71" t="str">
+      <c r="E12" s="71">
         <f>IF(_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E12)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G12)=0,"",_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$E12)+_xlfn.NUMBERVALUE('Sprint 2 - Bilan'!$G12))</f>
-        <v/>
-      </c>
-      <c r="F12" s="75" t="str">
+        <v>3.125E-2</v>
+      </c>
+      <c r="F12" s="75">
         <f>IF(LEN('Sprint 2 - Bilan'!$H12)&lt;&gt;0,'Sprint 2 - Bilan'!$H12,IF(LEN('Sprint 2 - Bilan'!$F12)=0,"",'Sprint 2 - Bilan'!$F12))</f>
-        <v/>
+        <v>1</v>
       </c>
       <c r="G12" s="110"/>
       <c r="H12" s="111"/>
       <c r="I12" s="112"/>
       <c r="M12" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="3" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="3" t="b">
         <f t="shared" si="2"/>
@@ -13219,7 +13235,7 @@
       </c>
       <c r="P12" s="3" t="b">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
@@ -13427,11 +13443,11 @@
       <c r="R16" s="8"/>
       <c r="V16" s="4">
         <f>P44</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="W16" s="4" t="str">
         <f>IF(V16=0,"",IF(V16=1,"Une tâche n'a pas été terminée!",CONCATENATE(V16," tâches n'ont pas été terminé!")))</f>
-        <v>25 tâches n'ont pas été terminé!</v>
+        <v>21 tâches n'ont pas été terminé!</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.25">
@@ -14571,11 +14587,11 @@
     <row r="44" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M44" s="3">
         <f>COUNTIF(M9:M43,TRUE)</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="N44" s="3">
         <f t="shared" ref="N44:O44" si="5">COUNTIF(N9:N43,TRUE)</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O44" s="3">
         <f t="shared" si="5"/>
@@ -14583,21 +14599,21 @@
       </c>
       <c r="P44" s="3">
         <f>COUNTIF(P9:P43,FALSE)</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="R44" s="8"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M45" s="3">
         <f>SUM(M44:O44)</f>
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="R45" s="8"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.25">
       <c r="M46" s="3" t="str">
         <f>IF(M45=0, "aucun champ", IF(M45=1, "1 champ", M45 &amp; " champs"))</f>
-        <v>50 champs</v>
+        <v>42 champs</v>
       </c>
       <c r="R46" s="8"/>
     </row>
@@ -14923,7 +14939,7 @@
       </c>
       <c r="C10" s="93" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>12h00</v>
       </c>
       <c r="D10" s="94" t="str">
         <f t="shared" si="0"/>
@@ -14935,13 +14951,13 @@
       </c>
       <c r="F10" s="99" t="str">
         <f t="shared" si="0"/>
-        <v>0h00</v>
+        <v>12h00</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="L10" s="1">
         <f>'Sprint 1 - Bilan'!T8</f>
-        <v>0</v>
+        <v>0.49999999999999967</v>
       </c>
       <c r="M10" s="1">
         <f>'Sprint 2 - Bilan'!V9</f>
@@ -14953,14 +14969,14 @@
       </c>
       <c r="O10" s="1">
         <f>SUM(L10:N10)</f>
-        <v>0</v>
+        <v>0.49999999999999967</v>
       </c>
       <c r="P10" s="1" t="s">
         <v>66</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="R10" s="1">
         <f t="shared" si="1"/>
@@ -14991,37 +15007,37 @@
       </c>
       <c r="C11" s="102">
         <f>L11</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D11" s="103">
         <f>M11</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E11" s="104">
         <f>N11</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F11" s="105">
         <f>O11</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="L11" s="1">
         <f>'Sprint 1 - Bilan'!T15</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M11" s="1">
         <f>'Sprint 2 - Bilan'!V16</f>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="N11" s="1">
         <f>'Sprint 3 - Bilan'!V16</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="O11" s="1">
         <f>N11</f>
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>

</xml_diff>